<commit_message>
new new 16a maggio
</commit_message>
<xml_diff>
--- a/prelievi.xlsx
+++ b/prelievi.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Data</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Scotch Magic</t>
+  </si>
+  <si>
+    <t>Rocche filo nero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocche filo bianco </t>
   </si>
 </sst>
 </file>
@@ -580,6 +586,57 @@
         <v>5</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="6">
+        <v>43235</v>
+      </c>
+      <c r="B22" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E22" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6">
+        <v>43235</v>
+      </c>
+      <c r="B23" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s" s="8">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E23" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6">
+        <v>43235</v>
+      </c>
+      <c r="B24" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E24" s="10">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new new 23 maggio
</commit_message>
<xml_diff>
--- a/prelievi.xlsx
+++ b/prelievi.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Data</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Centimetro</t>
+  </si>
+  <si>
+    <t>Silesia Nera</t>
   </si>
 </sst>
 </file>
@@ -763,6 +766,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="6">
+        <v>43243</v>
+      </c>
+      <c r="B31" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E31" s="10">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>